<commit_message>
Window to Show All Graceful Labelings is now working by displaying 1 graph in any location of the PictureBoxGraceful. It still needs to display all graceful labelings and each graph with corresponding edge label
</commit_message>
<xml_diff>
--- a/GraphTheoryEditor/CoordinatesConversion.xlsx
+++ b/GraphTheoryEditor/CoordinatesConversion.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Research\Graph Theory\Graceful\Find all graceful labels\GraphTheoryEditorWithFindAllGracefulLabelings\GraphTheoryEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F249DD4A-7653-4E8E-8337-9DDF9D07DB88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F509D44-B4B5-4180-BEDF-C0D53EF85B70}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="11895" xr2:uid="{1CB7BC10-CF0E-47D3-871E-42AE305A13AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="11895" activeTab="1" xr2:uid="{1CB7BC10-CF0E-47D3-871E-42AE305A13AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>y</t>
   </si>
@@ -62,12 +63,30 @@
   <si>
     <t>y'</t>
   </si>
+  <si>
+    <t>Rand x0</t>
+  </si>
+  <si>
+    <t>Rand x1</t>
+  </si>
+  <si>
+    <t>Rand y0</t>
+  </si>
+  <si>
+    <t>Rand y1</t>
+  </si>
+  <si>
+    <t>Xh</t>
+  </si>
+  <si>
+    <t>Yh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +94,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,13 +141,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Accent5" xfId="2" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,6 +1102,1461 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>244</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>633</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>519</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$B$2:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>438</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>323</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>368</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E9F0-44EF-B722-72FECC00AA6D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="510522160"/>
+        <c:axId val="510521504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="510522160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510521504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510521504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510522160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y'</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$M$2:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>433</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$N$2:$N$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>413</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6CF7-4EE4-B7F0-31A27C75803C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="510544464"/>
+        <c:axId val="510539544"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="510544464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510539544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="510539544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="510544464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sheet1 (2)'!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Yh</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$P$2:$P$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.79120879120879117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.52276295133437989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97174254317111464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16012558869701726</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8492935635792779E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5353218210361061E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12872841444270017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21664050235478807</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95447409733124022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56357927786499218</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.53061224489795922</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.7912087912087919E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.82731554160125587</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52590266875981162</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.2794348508634227E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.36106750392464676</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.60439560439560436</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.66562009419152279</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.47095761381475665</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.64835164835164838</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.67974882260596547</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.9827315541601257E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.14913657770800628</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.69387755102040816</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.82417582417582413</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.83987441130298268</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5698587127158557E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.81789638932496078</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.40031397174254318</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.9827315541601257E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.48822605965463106</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.67974882260596547</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sheet1 (2)'!$Q$2:$Q$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0.55952380952380953</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93809523809523809</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.72380952380952379</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55476190476190479</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78095238095238095</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1428571428571429E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98333333333333328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0476190476190474E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75714285714285712</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59523809523809523</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.73571428571428577</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.3880952380952381</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.18333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.48333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.22380952380952382</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.50714285714285712</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.49047619047619045</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.58809523809523812</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.23571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.52142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.16904761904761906</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.61428571428571432</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.88571428571428568</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98095238095238091</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.77857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.20238095238095238</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E7EC-44B2-9039-2FD5C92166E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="578815760"/>
+        <c:axId val="578817072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="578815760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="578817072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="578817072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="578815760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1125,6 +2637,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1642,6 +3274,1554 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2226,6 +5406,123 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>90486</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3141AF93-6C81-49A9-B8A4-5C07FE1F7A98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>138111</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{867E4133-8F0E-4048-AE6C-915711126CFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE025E5B-CA2A-47E6-8B58-DC1D2CC31FBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2533,8 +5830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E4AD12-8447-4433-AF2C-36C5A7DFD921}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,4 +6354,920 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3972D298-ED4D-431C-8C26-052961DEC99E}">
+  <dimension ref="A1:Q35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <v>800</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1">
+        <f>MIN(A2:A35)</f>
+        <v>106</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>610</v>
+      </c>
+      <c r="B2">
+        <v>345</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>600</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>MIN(B2:B35)</f>
+        <v>110</v>
+      </c>
+      <c r="M2">
+        <f>A2-$K$1</f>
+        <v>504</v>
+      </c>
+      <c r="N2">
+        <f>B2-$K$2</f>
+        <v>235</v>
+      </c>
+      <c r="P2">
+        <f>M2/($K$3-$K$1)</f>
+        <v>0.79120879120879117</v>
+      </c>
+      <c r="Q2">
+        <f>N2/($K$4-$K$2)</f>
+        <v>0.55952380952380953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>439</v>
+      </c>
+      <c r="B3">
+        <v>504</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>750</v>
+      </c>
+      <c r="J3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <f>MAX(A2:A35)</f>
+        <v>743</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M35" si="0">A3-$K$1</f>
+        <v>333</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N35" si="1">B3-$K$2</f>
+        <v>394</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P35" si="2">M3/($K$3-$K$1)</f>
+        <v>0.52276295133437989</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q35" si="3">N3/($K$4-$K$2)</f>
+        <v>0.93809523809523809</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>725</v>
+      </c>
+      <c r="B4">
+        <v>414</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4">
+        <v>550</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <f>MAX(B2:B35)</f>
+        <v>530</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>619</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="1"/>
+        <v>304</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>0.97174254317111464</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>0.72380952380952379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>208</v>
+      </c>
+      <c r="B5">
+        <v>343</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>102</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>233</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>0.16012558869701726</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>0.55476190476190479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>156</v>
+      </c>
+      <c r="B6">
+        <v>438</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>328</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>7.8492935635792779E-2</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>0.78095238095238095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>154</v>
+      </c>
+      <c r="B7">
+        <v>119</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>7.5353218210361061E-2</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>2.1428571428571429E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>188</v>
+      </c>
+      <c r="B8">
+        <v>530</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>0.12872841444270017</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>244</v>
+      </c>
+      <c r="B9">
+        <v>523</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>413</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>0.21664050235478807</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>0.98333333333333328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>714</v>
+      </c>
+      <c r="B10">
+        <v>148</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>608</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>0.95447409733124022</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>9.0476190476190474E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>465</v>
+      </c>
+      <c r="B11">
+        <v>188</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>359</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>0.56357927786499218</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>0.18571428571428572</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>444</v>
+      </c>
+      <c r="B12">
+        <v>446</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>338</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>0.53061224489795922</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>162</v>
+      </c>
+      <c r="B13">
+        <v>428</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>318</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>8.7912087912087919E-2</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="3"/>
+        <v>0.75714285714285712</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>633</v>
+      </c>
+      <c r="B14">
+        <v>360</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>527</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>0.82731554160125587</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="3"/>
+        <v>0.59523809523809523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>441</v>
+      </c>
+      <c r="B15">
+        <v>494</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>384</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="2"/>
+        <v>0.52590266875981162</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="3"/>
+        <v>0.91428571428571426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>110</v>
+      </c>
+      <c r="B16">
+        <v>419</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>309</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="2"/>
+        <v>6.2794348508634227E-3</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="3"/>
+        <v>0.73571428571428577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>336</v>
+      </c>
+      <c r="B17">
+        <v>348</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>230</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>238</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="2"/>
+        <v>0.36106750392464676</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="3"/>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>491</v>
+      </c>
+      <c r="B18">
+        <v>273</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>385</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="2"/>
+        <v>0.60439560439560436</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="3"/>
+        <v>0.3880952380952381</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>530</v>
+      </c>
+      <c r="B19">
+        <v>187</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>424</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="2"/>
+        <v>0.66562009419152279</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="3"/>
+        <v>0.18333333333333332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>106</v>
+      </c>
+      <c r="B20">
+        <v>446</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>406</v>
+      </c>
+      <c r="B21">
+        <v>313</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>203</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>0.47095761381475665</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="3"/>
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>743</v>
+      </c>
+      <c r="B22">
+        <v>204</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>637</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="3"/>
+        <v>0.22380952380952382</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>519</v>
+      </c>
+      <c r="B23">
+        <v>323</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>413</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>213</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>0.64835164835164838</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="3"/>
+        <v>0.50714285714285712</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>539</v>
+      </c>
+      <c r="B24">
+        <v>316</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>433</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>0.67974882260596547</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="3"/>
+        <v>0.49047619047619045</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>125</v>
+      </c>
+      <c r="B25">
+        <v>357</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>247</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>2.9827315541601257E-2</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="3"/>
+        <v>0.58809523809523812</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>201</v>
+      </c>
+      <c r="B26">
+        <v>209</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>0.14913657770800628</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="3"/>
+        <v>0.23571428571428571</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>548</v>
+      </c>
+      <c r="B27">
+        <v>329</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>442</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>0.69387755102040816</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="3"/>
+        <v>0.52142857142857146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>631</v>
+      </c>
+      <c r="B28">
+        <v>181</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>0.82417582417582413</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="3"/>
+        <v>0.16904761904761906</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>641</v>
+      </c>
+      <c r="B29">
+        <v>110</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="0"/>
+        <v>535</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>0.83987441130298268</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>107</v>
+      </c>
+      <c r="B30">
+        <v>368</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>258</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="2"/>
+        <v>1.5698587127158557E-3</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="3"/>
+        <v>0.61428571428571432</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>627</v>
+      </c>
+      <c r="B31">
+        <v>482</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="0"/>
+        <v>521</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>372</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="2"/>
+        <v>0.81789638932496078</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="3"/>
+        <v>0.88571428571428568</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>361</v>
+      </c>
+      <c r="B32">
+        <v>522</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>255</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>412</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="2"/>
+        <v>0.40031397174254318</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="3"/>
+        <v>0.98095238095238091</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>125</v>
+      </c>
+      <c r="B33">
+        <v>437</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>327</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="2"/>
+        <v>2.9827315541601257E-2</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="3"/>
+        <v>0.77857142857142858</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>417</v>
+      </c>
+      <c r="B34">
+        <v>306</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="0"/>
+        <v>311</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>0.48822605965463106</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="3"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>539</v>
+      </c>
+      <c r="B35">
+        <v>195</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="0"/>
+        <v>433</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>0.67974882260596547</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="3"/>
+        <v>0.20238095238095238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>